<commit_message>
fix: degree C title in bbExcel
</commit_message>
<xml_diff>
--- a/excels/BB_ExcelForm.xlsx
+++ b/excels/BB_ExcelForm.xlsx
@@ -221,25 +221,7 @@
     <t>Lít</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t>C</t>
-    </r>
+    <t>Độ C</t>
   </si>
   <si>
     <t>%</t>
@@ -310,13 +292,6 @@
     </font>
     <font>
       <sz val="13"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
@@ -486,6 +461,13 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
@@ -685,7 +667,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -919,6 +901,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="hair">
         <color auto="1"/>
@@ -1080,133 +1077,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1353,7 +1350,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1386,11 +1383,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1401,6 +1395,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1467,7 +1464,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1476,7 +1473,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="179" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3309,8 +3306,8 @@
   <sheetPr/>
   <dimension ref="A1:BB100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="AK22" sqref="AK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.85714285714286" defaultRowHeight="19.5" customHeight="1"/>
@@ -4725,11 +4722,11 @@
         <v>43</v>
       </c>
       <c r="P31" s="26"/>
-      <c r="Q31" s="40"/>
+      <c r="Q31" s="26"/>
       <c r="R31" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="S31" s="27"/>
+      <c r="S31" s="48"/>
       <c r="T31" s="25" t="s">
         <v>43</v>
       </c>
@@ -4746,11 +4743,11 @@
         <v>43</v>
       </c>
       <c r="AC31" s="26"/>
-      <c r="AD31" s="40"/>
+      <c r="AD31" s="26"/>
       <c r="AE31" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="AF31" s="27"/>
+      <c r="AF31" s="48"/>
       <c r="AG31" s="25" t="s">
         <v>45</v>
       </c>

</xml_diff>